<commit_message>
validations are working for csv file need to merge in master
</commit_message>
<xml_diff>
--- a/bills.xlsx
+++ b/bills.xlsx
@@ -71,7 +71,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -93,6 +93,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,8 +143,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -162,7 +172,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -212,7 +222,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>7015</v>
+        <v>7060</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>11</v>
@@ -241,7 +251,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>7016</v>
+        <v>7061</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>11</v>
@@ -255,8 +265,8 @@
       <c r="H3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>51</v>
+      <c r="I3" s="1" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,7 +280,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>7017</v>
+        <v>7062</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>11</v>
@@ -285,7 +295,7 @@
         <v>14</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -299,7 +309,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>7018</v>
+        <v>7063</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>11</v>
@@ -314,7 +324,7 @@
         <v>14</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -328,7 +338,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>7015</v>
+        <v>7064</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
new bills are added
</commit_message>
<xml_diff>
--- a/bills.xlsx
+++ b/bills.xlsx
@@ -222,7 +222,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>7060</v>
+        <v>7080</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>11</v>
@@ -251,7 +251,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>7061</v>
+        <v>7081</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>11</v>
@@ -280,7 +280,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>7062</v>
+        <v>7082</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>11</v>
@@ -309,7 +309,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>7063</v>
+        <v>7083</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>11</v>
@@ -338,7 +338,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>7064</v>
+        <v>7084</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
added bundle no validation for bill model
</commit_message>
<xml_diff>
--- a/bills.xlsx
+++ b/bills.xlsx
@@ -172,7 +172,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -222,7 +222,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>7060</v>
+        <v>7080</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>11</v>
@@ -251,7 +251,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>7061</v>
+        <v>7021</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>11</v>
@@ -280,7 +280,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>7062</v>
+        <v>7022</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>11</v>
@@ -309,7 +309,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>7063</v>
+        <v>7023</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>11</v>
@@ -338,7 +338,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>7064</v>
+        <v>7024</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
for testing used bill csv file
</commit_message>
<xml_diff>
--- a/bills.xlsx
+++ b/bills.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>section</t>
   </si>
@@ -58,10 +58,7 @@
     <t>A</t>
   </si>
   <si>
-    <t> A1</t>
-  </si>
-  <si>
-    <t>A4</t>
+    <t>A1</t>
   </si>
 </sst>
 </file>
@@ -71,7 +68,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -93,12 +90,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,12 +134,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -169,7 +156,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
@@ -222,7 +209,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>7080</v>
+        <v>8010</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>11</v>
@@ -237,122 +224,6 @@
         <v>13</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>2015</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>7021</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>2015</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>7022</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>2015</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>7023</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>2015</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>7024</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="0" t="n">
         <v>52</v>
       </c>
     </row>

</xml_diff>